<commit_message>
Alhamdulillah, completed until the part where 'resolve' button is clickable.
</commit_message>
<xml_diff>
--- a/Case_data.xlsx
+++ b/Case_data.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Rough" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Vendor Code</t>
   </si>
@@ -36,6 +37,9 @@
   </si>
   <si>
     <t>34EUN</t>
+  </si>
+  <si>
+    <t>Made Changes</t>
   </si>
 </sst>
 </file>
@@ -353,20 +357,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -376,8 +379,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -386,9 +392,24 @@
       </c>
       <c r="C2">
         <v>9</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Alhamdulillah, completed to the entire code. Only loop is pending.
</commit_message>
<xml_diff>
--- a/Case_data.xlsx
+++ b/Case_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Vendor Code</t>
   </si>
@@ -41,12 +41,18 @@
   <si>
     <t>Made Changes</t>
   </si>
+  <si>
+    <t>Mention Login ID Below</t>
+  </si>
+  <si>
+    <t>mmohdat</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,16 +60,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9997B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -71,18 +113,150 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF9997B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -357,48 +531,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>490769</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="2">
+        <v>514766</v>
+      </c>
+      <c r="C2" s="2">
         <v>9</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>5</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G2:I4"/>
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Alhamdulillah, completed to the entire code with explecit waits.
</commit_message>
<xml_diff>
--- a/Case_data.xlsx
+++ b/Case_data.xlsx
@@ -36,9 +36,6 @@
     <t>No of ASINs</t>
   </si>
   <si>
-    <t>34EUN</t>
-  </si>
-  <si>
     <t>Made Changes</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>mmohdat</t>
+  </si>
+  <si>
+    <t>FATKP</t>
   </si>
 </sst>
 </file>
@@ -533,9 +533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -556,29 +554,29 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>5</v>
       </c>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>518219</v>
+      </c>
+      <c r="C2" s="2">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>514766</v>
-      </c>
-      <c r="C2" s="2">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="G2" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>

</xml_diff>

<commit_message>
Alhamdulillah, completed the entire script with updated excel.
</commit_message>
<xml_diff>
--- a/Case_data.xlsx
+++ b/Case_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Vendor Code</t>
   </si>
@@ -47,21 +47,23 @@
   <si>
     <t>FATKP</t>
   </si>
+  <si>
+    <t>Mention Correspondence Below</t>
+  </si>
+  <si>
+    <t>Hi,
+We are informing you that this task is for RBS use only and has been raised to track Proactive Work. We have reviewed &amp; corrected ASINs in the attachment. 
+Winston tool is automatically linking this vendor code with corresponding BS, however, no action is required from BS side. 
+Thanks, 
+Mohammed Ataullah</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,8 +86,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +122,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3F3F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -212,39 +236,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -254,6 +292,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF3F3F"/>
+      <color rgb="FFF1E145"/>
       <color rgb="FFF9997B"/>
     </mruColors>
   </colors>
@@ -531,29 +571,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9:P23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="12" t="s">
@@ -562,17 +605,17 @@
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>518219</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>6</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -581,20 +624,221 @@
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G3" s="6"/>
       <c r="H3" s="7"/>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G4" s="9"/>
       <c r="H4" s="10"/>
       <c r="I4" s="11"/>
     </row>
+    <row r="8" spans="1:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="G8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+    </row>
+    <row r="9" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+    </row>
+    <row r="10" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+    </row>
+    <row r="11" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+    </row>
+    <row r="14" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+    </row>
+    <row r="15" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+    </row>
+    <row r="17" spans="7:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+    </row>
+    <row r="18" spans="7:16" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+    </row>
+    <row r="19" spans="7:16" x14ac:dyDescent="0.35">
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+    </row>
+    <row r="20" spans="7:16" x14ac:dyDescent="0.35">
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+    </row>
+    <row r="21" spans="7:16" x14ac:dyDescent="0.35">
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+    </row>
+    <row r="22" spans="7:16" x14ac:dyDescent="0.35">
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+    </row>
+    <row r="23" spans="7:16" x14ac:dyDescent="0.35">
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+    </row>
+    <row r="24" spans="7:16" x14ac:dyDescent="0.35">
+      <c r="G24" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="G2:I4"/>
     <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G9:P23"/>
+    <mergeCell ref="G8:P8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Alhamdulillah, results can be known in excel sheet also now.
</commit_message>
<xml_diff>
--- a/Case_data.xlsx
+++ b/Case_data.xlsx
@@ -13,19 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Rough" sheetId="2" r:id="rId2"/>
+    <sheet name="Result" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Vendor Code</t>
   </si>
@@ -42,10 +37,10 @@
     <t>Mention Login ID Below</t>
   </si>
   <si>
+    <t>MSAO5</t>
+  </si>
+  <si>
     <t>mmohdat</t>
-  </si>
-  <si>
-    <t>FATKP</t>
   </si>
   <si>
     <t>Mention Correspondence Below</t>
@@ -56,6 +51,9 @@
 Winston tool is automatically linking this vendor code with corresponding BS, however, no action is required from BS side. 
 Thanks, 
 Mohammed Ataullah</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -129,7 +127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -153,17 +151,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -232,57 +219,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -290,13 +285,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FFFF3F3F"/>
-      <color rgb="FFF1E145"/>
-      <color rgb="FFF9997B"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -575,263 +563,265 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9:P23"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:16" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>518748</v>
+      </c>
+      <c r="C2" s="3">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
-        <v>518219</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="D2" s="3">
+        <v>3</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
-        <v>3</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="8" spans="1:16" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="G8" s="13" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="8" spans="1:16" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" spans="7:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" spans="7:16" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
     </row>
     <row r="23" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
     </row>
     <row r="24" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G24" s="15"/>
+      <c r="G24" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -841,18 +831,35 @@
     <mergeCell ref="G8:P8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Alhamdulillah, 'Ok' button has been fixed.
</commit_message>
<xml_diff>
--- a/Case_data.xlsx
+++ b/Case_data.xlsx
@@ -14,13 +14,14 @@
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Result" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Vendor Code</t>
   </si>
@@ -37,30 +38,38 @@
     <t>Mention Login ID Below</t>
   </si>
   <si>
-    <t>MSAO5</t>
-  </si>
-  <si>
     <t>mmohdat</t>
   </si>
   <si>
     <t>Mention Correspondence Below</t>
   </si>
   <si>
-    <t>Hi,
-We are informing you that this task is for RBS use only and has been raised to track Proactive Work. We have reviewed &amp; corrected ASINs in the attachment. 
-Winston tool is automatically linking this vendor code with corresponding BS, however, no action is required from BS side. 
-Thanks, 
-Mohammed Ataullah</t>
+    <t>Automation Script Testing</t>
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>34EUN</t>
+  </si>
+  <si>
+    <t>JPXB0</t>
+  </si>
+  <si>
+    <t>MJ0XQ</t>
+  </si>
+  <si>
+    <t>NIKE5</t>
+  </si>
+  <si>
+    <t>NUKP5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +109,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -247,11 +264,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -276,9 +296,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,10 +586,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -587,238 +605,274 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4">
+        <v>562248</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3">
-        <v>518748</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4">
+        <v>562252</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4">
+        <v>562256</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4">
+        <v>562258</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="F4" s="3"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="8" spans="1:16" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G8" s="17" t="s">
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+    </row>
+    <row r="9" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-    </row>
-    <row r="9" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G9" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
     </row>
     <row r="11" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
     </row>
     <row r="13" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
     </row>
     <row r="14" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
     </row>
     <row r="15" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
     </row>
     <row r="16" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
     </row>
     <row r="17" spans="7:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
     </row>
     <row r="18" spans="7:16" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
     </row>
     <row r="19" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
     </row>
     <row r="20" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
     </row>
     <row r="21" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
     </row>
     <row r="22" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
     </row>
     <row r="23" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
     </row>
     <row r="24" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G24" s="2"/>
@@ -837,29 +891,81 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>9</v>
-      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B2"/>
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3"/>
+      <c r="C3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>562235</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Alhamdulillah, Script is working correctly now.
</commit_message>
<xml_diff>
--- a/Case_data.xlsx
+++ b/Case_data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
   <si>
     <t>Vendor Code</t>
   </si>
@@ -38,9 +38,30 @@
     <t>Mention Login ID Below</t>
   </si>
   <si>
+    <t>RAZ3T</t>
+  </si>
+  <si>
     <t>mmohdat</t>
   </si>
   <si>
+    <t>BLAMT</t>
+  </si>
+  <si>
+    <t>EILL5</t>
+  </si>
+  <si>
+    <t>ENWO5</t>
+  </si>
+  <si>
+    <t>KNIPW</t>
+  </si>
+  <si>
+    <t>ELXA5</t>
+  </si>
+  <si>
+    <t>ELUZ5</t>
+  </si>
+  <si>
     <t>Mention Correspondence Below</t>
   </si>
   <si>
@@ -50,6 +71,9 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Resolved</t>
+  </si>
+  <si>
     <t>34EUN</t>
   </si>
   <si>
@@ -63,6 +87,30 @@
   </si>
   <si>
     <t>NUKP5</t>
+  </si>
+  <si>
+    <t>HAGBN</t>
+  </si>
+  <si>
+    <t>FATKP</t>
+  </si>
+  <si>
+    <t>SYSAN</t>
+  </si>
+  <si>
+    <t>INULF</t>
+  </si>
+  <si>
+    <t>KELEJ</t>
+  </si>
+  <si>
+    <t>KREBG</t>
+  </si>
+  <si>
+    <t>INTW5</t>
+  </si>
+  <si>
+    <t>KEBK5</t>
   </si>
 </sst>
 </file>
@@ -273,6 +321,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -296,7 +345,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,10 +634,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -605,274 +653,224 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="4">
-        <v>562248</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
+      <c r="G2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="4">
-        <v>562252</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="4">
-        <v>562256</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="8" spans="1:16" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4">
-        <v>562258</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G8" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
     </row>
     <row r="9" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G9" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
+      <c r="G9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
     </row>
     <row r="10" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
     </row>
     <row r="11" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
     </row>
     <row r="13" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
     </row>
     <row r="14" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
     </row>
     <row r="15" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
     </row>
     <row r="16" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
     </row>
     <row r="17" spans="7:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
     </row>
     <row r="18" spans="7:16" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
     </row>
     <row r="19" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
     </row>
     <row r="20" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
     </row>
     <row r="21" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
     </row>
     <row r="22" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
     </row>
     <row r="23" spans="7:16" x14ac:dyDescent="0.35">
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
     </row>
     <row r="24" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G24" s="2"/>
@@ -891,15 +889,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.4">
@@ -910,16 +910,85 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>562283</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>562286</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B2"/>
-      <c r="C2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B3"/>
-      <c r="C3"/>
+      <c r="B4">
+        <v>562287</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>562289</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>562379</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>562380</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>562384</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -928,31 +997,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>562235</v>
@@ -963,9 +1030,335 @@
       <c r="D2">
         <v>0</v>
       </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>562248</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>562252</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>562256</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>562258</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>562260</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>562263</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>562266</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>562270</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <v>562272</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>562274</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>562283</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>562286</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>562287</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>562289</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>562379</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>562380</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <v>562384</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>562386</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>562388</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>